<commit_message>
Added to precis of Burke's Reflections
</commit_message>
<xml_diff>
--- a/recite_hooker.xlsx
+++ b/recite_hooker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>3/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,10 @@
   </si>
   <si>
     <t>4/4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If it be granted a thing unlawful for private men, not called unto public consultation, to dispute which is the best state of civil polity,(with a desire of bringing in some other kind, than that under which they already live, for of such disputes I take it his meaning was;)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,7 +440,7 @@
   <dimension ref="B2:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -496,6 +500,9 @@
       <c r="C6" s="4">
         <v>43325</v>
       </c>
+      <c r="D6" s="4">
+        <v>43326</v>
+      </c>
     </row>
     <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -504,9 +511,17 @@
       <c r="C7" s="4">
         <v>43325</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B8" s="1"/>
+      <c r="D7" s="4">
+        <v>43326</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="75" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43326</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
Updated precis_burke and recite_hooker
</commit_message>
<xml_diff>
--- a/recite_hooker.xlsx
+++ b/recite_hooker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>3/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,10 @@
   </si>
   <si>
     <t>When they which write in defence of your discipline and commend it unto the Highest not in the least cunning manner, are forced notwithstanding to acknowledge, "that with whom the truth is they know not," they are not certain; what certainty or knowledge can the multitude have thereof?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weigh what doth move the common sort so much to favour this innovation, and it shall soon appear unto you, that the force of particular reasons which for your several opinions are alleged is a thing whereof the multitude never did nor could so consider as to be therewith wholly carried; but certain general inducements are used to make them more saleable your cause in gross;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -533,6 +537,9 @@
       <c r="J6" s="4">
         <v>43333</v>
       </c>
+      <c r="K6" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
@@ -562,6 +569,9 @@
       <c r="J7" s="4">
         <v>43333</v>
       </c>
+      <c r="K7" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="8" spans="2:14" ht="75" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
@@ -588,6 +598,9 @@
       <c r="I8" s="4">
         <v>43333</v>
       </c>
+      <c r="J8" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="9" spans="2:14" ht="60" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
@@ -611,6 +624,9 @@
       <c r="H9" s="4">
         <v>43333</v>
       </c>
+      <c r="I9" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="10" spans="2:14" ht="75" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
@@ -631,6 +647,9 @@
       <c r="G10" s="4">
         <v>43333</v>
       </c>
+      <c r="H10" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="11" spans="2:14" ht="75" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
@@ -648,9 +667,17 @@
       <c r="F11" s="4">
         <v>43333</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B12" s="1"/>
+      <c r="G11" s="4">
+        <v>43334</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="90" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4">
+        <v>43334</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B13" s="1"/>

</xml_diff>